<commit_message>
North Macedonia data entered
</commit_message>
<xml_diff>
--- a/data/simplifiedData2021.xlsx
+++ b/data/simplifiedData2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanscassellati/Data_Visualization/Project/cosi-116a-f24-final-project-repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B89AA18-FC0C-2644-859F-194261246152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7358F772-59EC-6541-B908-64450E05229A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="13820" windowHeight="14340" xr2:uid="{28DD3533-A644-B740-9E1F-02EA1467CA1F}"/>
+    <workbookView xWindow="10600" yWindow="500" windowWidth="13820" windowHeight="14340" xr2:uid="{28DD3533-A644-B740-9E1F-02EA1467CA1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
   <si>
     <t>Renewable2021</t>
   </si>
@@ -1335,6 +1335,12 @@
   </si>
   <si>
     <t>CountryID</t>
+  </si>
+  <si>
+    <t>MKD</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
   </si>
 </sst>
 </file>
@@ -1713,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541C9CC-3DC3-A74E-9432-2834F1B0C62F}">
-  <dimension ref="A1:E215"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C215" sqref="C215"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5382,6 +5388,23 @@
         <v>431</v>
       </c>
     </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>19.48</v>
+      </c>
+      <c r="B216">
+        <v>100</v>
+      </c>
+      <c r="C216">
+        <v>807</v>
+      </c>
+      <c r="D216" t="s">
+        <v>434</v>
+      </c>
+      <c r="E216" t="s">
+        <v>433</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D249">
     <sortCondition ref="D2:D249"/>

</xml_diff>

<commit_message>
adding correct data to map and cleaning data
</commit_message>
<xml_diff>
--- a/data/simplifiedData2021.xlsx
+++ b/data/simplifiedData2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanscassellati/Data_Visualization/Project/cosi-116a-f24-final-project-repository/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinegorey/Documents/COSI116A/cosi-116a-f24-final-project-repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B89AA18-FC0C-2644-859F-194261246152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9370CFE-7FAF-7043-A3BF-7EFB1CFB3E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="13820" windowHeight="14340" xr2:uid="{28DD3533-A644-B740-9E1F-02EA1467CA1F}"/>
+    <workbookView xWindow="2140" yWindow="3240" windowWidth="13820" windowHeight="14340" xr2:uid="{28DD3533-A644-B740-9E1F-02EA1467CA1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1334,7 +1334,7 @@
     <t>ZWE</t>
   </si>
   <si>
-    <t>CountryID</t>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1715,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541C9CC-3DC3-A74E-9432-2834F1B0C62F}">
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C215" sqref="C215"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
data cleaning and addition for continents data
</commit_message>
<xml_diff>
--- a/data/simplifiedData2021.xlsx
+++ b/data/simplifiedData2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinegorey/Documents/COSI116A/cosi-116a-f24-final-project-repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01096ECE-C767-014A-8ADD-E367B15005F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF36A765-B57A-6A45-AA2F-27D1D02261DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="2080" windowWidth="13820" windowHeight="14340" xr2:uid="{28DD3533-A644-B740-9E1F-02EA1467CA1F}"/>
+    <workbookView xWindow="7980" yWindow="2040" windowWidth="13820" windowHeight="14340" xr2:uid="{28DD3533-A644-B740-9E1F-02EA1467CA1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="448">
   <si>
     <t>Renewable2021</t>
   </si>
@@ -1355,17 +1355,38 @@
     <t>CIV</t>
   </si>
   <si>
-    <t>Cote d'Ivoire</t>
-  </si>
-  <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>Continent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1384,6 +1405,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1406,10 +1445,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1744,21 +1786,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541C9CC-3DC3-A74E-9432-2834F1B0C62F}">
-  <dimension ref="A1:E219"/>
+  <dimension ref="A1:F219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1772,10 +1815,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>19.98</v>
       </c>
@@ -1791,8 +1837,11 @@
       <c r="E2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>41.91</v>
       </c>
@@ -1808,8 +1857,11 @@
       <c r="E3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>0.12</v>
       </c>
@@ -1825,8 +1877,11 @@
       <c r="E4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>0.39</v>
       </c>
@@ -1842,8 +1897,11 @@
       <c r="E5" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>18.39</v>
       </c>
@@ -1859,8 +1917,11 @@
       <c r="E6" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>52.88</v>
       </c>
@@ -1876,8 +1937,11 @@
       <c r="E7" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>0.77</v>
       </c>
@@ -1893,8 +1957,11 @@
       <c r="E8" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>0.9</v>
       </c>
@@ -1910,8 +1977,11 @@
       <c r="E9" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9.24</v>
       </c>
@@ -1927,8 +1997,11 @@
       <c r="E10" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>9.1300000000000008</v>
       </c>
@@ -1944,8 +2017,11 @@
       <c r="E11" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>8.76</v>
       </c>
@@ -1961,8 +2037,11 @@
       <c r="E12" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12.32</v>
       </c>
@@ -1978,8 +2057,11 @@
       <c r="E13" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>36</v>
       </c>
@@ -1995,8 +2077,11 @@
       <c r="E14" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>1.32</v>
       </c>
@@ -2012,8 +2097,11 @@
       <c r="E15" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>1.1100000000000001</v>
       </c>
@@ -2029,8 +2117,11 @@
       <c r="E16" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>0.02</v>
       </c>
@@ -2046,8 +2137,11 @@
       <c r="E17" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>25.04</v>
       </c>
@@ -2063,8 +2157,11 @@
       <c r="E18" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>5.46</v>
       </c>
@@ -2080,8 +2177,11 @@
       <c r="E19" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>8.2200000000000006</v>
       </c>
@@ -2097,8 +2197,11 @@
       <c r="E20" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>11.68</v>
       </c>
@@ -2114,8 +2217,11 @@
       <c r="E21" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>26.56</v>
       </c>
@@ -2131,8 +2237,11 @@
       <c r="E22" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>54.52</v>
       </c>
@@ -2148,8 +2257,11 @@
       <c r="E23" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>0.9</v>
       </c>
@@ -2165,8 +2277,11 @@
       <c r="E24" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>81.81</v>
       </c>
@@ -2182,8 +2297,11 @@
       <c r="E25" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>12.76</v>
       </c>
@@ -2199,8 +2317,11 @@
       <c r="E26" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>36.61</v>
       </c>
@@ -2216,8 +2337,11 @@
       <c r="E27" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>27.36</v>
       </c>
@@ -2233,8 +2357,11 @@
       <c r="E28" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>46.48</v>
       </c>
@@ -2250,8 +2377,11 @@
       <c r="E29" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>0.03</v>
       </c>
@@ -2267,8 +2397,11 @@
       <c r="E30" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>20.38</v>
       </c>
@@ -2284,8 +2417,11 @@
       <c r="E31" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>71.16</v>
       </c>
@@ -2301,8 +2437,11 @@
       <c r="E32" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>83.14</v>
       </c>
@@ -2318,8 +2457,11 @@
       <c r="E33" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>22.64</v>
       </c>
@@ -2335,8 +2477,11 @@
       <c r="E34" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>52.38</v>
       </c>
@@ -2352,8 +2497,11 @@
       <c r="E35" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>79.239999999999995</v>
       </c>
@@ -2369,8 +2517,11 @@
       <c r="E36" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>23.84</v>
       </c>
@@ -2386,8 +2537,11 @@
       <c r="E37" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>0.01</v>
       </c>
@@ -2403,8 +2557,11 @@
       <c r="E38" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>90.92</v>
       </c>
@@ -2420,8 +2577,11 @@
       <c r="E39" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>69.900000000000006</v>
       </c>
@@ -2437,8 +2597,11 @@
       <c r="E40" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>24.17</v>
       </c>
@@ -2454,8 +2617,11 @@
       <c r="E41" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>15.21</v>
       </c>
@@ -2471,8 +2637,11 @@
       <c r="E42" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>29.7</v>
       </c>
@@ -2488,8 +2657,11 @@
       <c r="E43" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>41.19</v>
       </c>
@@ -2505,8 +2677,11 @@
       <c r="E44" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>71.38</v>
       </c>
@@ -2522,8 +2697,11 @@
       <c r="E45" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>8.76</v>
       </c>
@@ -2539,8 +2717,11 @@
       <c r="E46" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>34.159999999999997</v>
       </c>
@@ -2556,8 +2737,11 @@
       <c r="E47" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>34.07</v>
       </c>
@@ -2573,8 +2757,11 @@
       <c r="E48" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>20.91</v>
       </c>
@@ -2590,8 +2777,11 @@
       <c r="E49" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>2.75</v>
       </c>
@@ -2607,8 +2797,11 @@
       <c r="E50" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>15.63</v>
       </c>
@@ -2624,8 +2817,11 @@
       <c r="E51" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>17.16</v>
       </c>
@@ -2641,8 +2837,11 @@
       <c r="E52" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>14.72</v>
       </c>
@@ -2658,8 +2857,11 @@
       <c r="E53" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>96.33</v>
       </c>
@@ -2675,8 +2877,11 @@
       <c r="E54" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>39.520000000000003</v>
       </c>
@@ -2692,8 +2897,11 @@
       <c r="E55" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>26.56</v>
       </c>
@@ -2709,8 +2917,11 @@
       <c r="E56" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>8.83</v>
       </c>
@@ -2726,8 +2937,11 @@
       <c r="E57" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>14.82</v>
       </c>
@@ -2743,8 +2957,11 @@
       <c r="E58" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>18.899999999999999</v>
       </c>
@@ -2760,8 +2977,11 @@
       <c r="E59" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>6.11</v>
       </c>
@@ -2777,8 +2997,11 @@
       <c r="E60" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>21.91</v>
       </c>
@@ -2794,8 +3017,11 @@
       <c r="E61" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>5.25</v>
       </c>
@@ -2811,8 +3037,11 @@
       <c r="E62" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>80.66</v>
       </c>
@@ -2828,8 +3057,11 @@
       <c r="E63" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>37.979999999999997</v>
       </c>
@@ -2845,8 +3077,11 @@
       <c r="E64" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>65.400000000000006</v>
       </c>
@@ -2862,8 +3097,11 @@
       <c r="E65" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>90.63</v>
       </c>
@@ -2879,8 +3117,11 @@
       <c r="E66" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>5.08</v>
       </c>
@@ -2896,8 +3137,11 @@
       <c r="E67" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>29.7</v>
       </c>
@@ -2913,8 +3157,11 @@
       <c r="E68" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>50.22</v>
       </c>
@@ -2930,8 +3177,11 @@
       <c r="E69" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>16.25</v>
       </c>
@@ -2947,8 +3197,11 @@
       <c r="E70" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>7.44</v>
       </c>
@@ -2964,8 +3217,11 @@
       <c r="E71" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>91.27</v>
       </c>
@@ -2981,8 +3237,11 @@
       <c r="E72" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>48.58</v>
       </c>
@@ -2998,8 +3257,11 @@
       <c r="E73" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>25.18</v>
       </c>
@@ -3015,8 +3277,11 @@
       <c r="E74" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>17.61</v>
       </c>
@@ -3032,8 +3297,11 @@
       <c r="E75" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76">
         <v>39.049999999999997</v>
       </c>
@@ -3049,8 +3317,11 @@
       <c r="E76" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77">
         <v>0</v>
       </c>
@@ -3066,8 +3337,11 @@
       <c r="E77" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78">
         <v>21.47</v>
       </c>
@@ -3083,8 +3357,11 @@
       <c r="E78" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79">
         <v>11.64</v>
       </c>
@@ -3100,8 +3377,11 @@
       <c r="E79" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80">
         <v>10.220000000000001</v>
       </c>
@@ -3117,8 +3397,11 @@
       <c r="E80" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81">
         <v>4.5</v>
       </c>
@@ -3134,8 +3417,11 @@
       <c r="E81" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82">
         <v>62.13</v>
       </c>
@@ -3151,8 +3437,11 @@
       <c r="E82" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83">
         <v>66.849999999999994</v>
       </c>
@@ -3168,8 +3457,11 @@
       <c r="E83" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84">
         <v>87.37</v>
       </c>
@@ -3185,8 +3477,11 @@
       <c r="E84" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85">
         <v>13.2</v>
       </c>
@@ -3202,8 +3497,11 @@
       <c r="E85" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86">
         <v>76.72</v>
       </c>
@@ -3219,8 +3517,11 @@
       <c r="E86" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87">
         <v>45.91</v>
       </c>
@@ -3236,8 +3537,11 @@
       <c r="E87" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88">
         <v>0.42</v>
       </c>
@@ -3253,8 +3557,11 @@
       <c r="E88" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89">
         <v>15.3</v>
       </c>
@@ -3270,8 +3577,11 @@
       <c r="E89" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90">
         <v>82.43</v>
       </c>
@@ -3287,8 +3597,11 @@
       <c r="E90" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91">
         <v>34.92</v>
       </c>
@@ -3304,8 +3617,11 @@
       <c r="E91" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92">
         <v>20.190000000000001</v>
       </c>
@@ -3321,8 +3637,11 @@
       <c r="E92" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93">
         <v>0.91</v>
       </c>
@@ -3338,8 +3657,11 @@
       <c r="E93" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94">
         <v>1.1000000000000001</v>
       </c>
@@ -3355,8 +3677,11 @@
       <c r="E94" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95">
         <v>12.69</v>
       </c>
@@ -3372,8 +3697,11 @@
       <c r="E95" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96">
         <v>3.16</v>
       </c>
@@ -3389,8 +3717,11 @@
       <c r="E96" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97">
         <v>6.2</v>
       </c>
@@ -3406,8 +3737,11 @@
       <c r="E97" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98">
         <v>17.54</v>
       </c>
@@ -3423,8 +3757,11 @@
       <c r="E98" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99">
         <v>10.49</v>
       </c>
@@ -3440,8 +3777,11 @@
       <c r="E99" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100">
         <v>8.84</v>
       </c>
@@ -3457,8 +3797,11 @@
       <c r="E100" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101">
         <v>11.5</v>
       </c>
@@ -3474,8 +3817,11 @@
       <c r="E101" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102">
         <v>1.99</v>
       </c>
@@ -3491,8 +3837,11 @@
       <c r="E102" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103">
         <v>67.67</v>
       </c>
@@ -3508,8 +3857,11 @@
       <c r="E103" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104">
         <v>42.23</v>
       </c>
@@ -3525,8 +3877,11 @@
       <c r="E104" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -3542,8 +3897,11 @@
       <c r="E105" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106">
         <v>27.63</v>
       </c>
@@ -3559,8 +3917,11 @@
       <c r="E106" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107">
         <v>51.53</v>
       </c>
@@ -3576,8 +3937,11 @@
       <c r="E107" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108">
         <v>43.99</v>
       </c>
@@ -3593,8 +3957,11 @@
       <c r="E108" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109">
         <v>6.82</v>
       </c>
@@ -3610,8 +3977,11 @@
       <c r="E109" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110">
         <v>33.630000000000003</v>
       </c>
@@ -3627,8 +3997,11 @@
       <c r="E110" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111">
         <v>93.19</v>
       </c>
@@ -3644,8 +4017,11 @@
       <c r="E111" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112">
         <v>3.12</v>
       </c>
@@ -3661,8 +4037,11 @@
       <c r="E112" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113">
         <v>53.61</v>
       </c>
@@ -3678,8 +4057,11 @@
       <c r="E113" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114">
         <v>33.22</v>
       </c>
@@ -3695,8 +4077,11 @@
       <c r="E114" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115">
         <v>20.51</v>
       </c>
@@ -3712,8 +4097,11 @@
       <c r="E115" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116">
         <v>83.61</v>
       </c>
@@ -3729,8 +4117,11 @@
       <c r="E116" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117">
         <v>71.08</v>
       </c>
@@ -3746,8 +4137,11 @@
       <c r="E117" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118">
         <v>7.48</v>
       </c>
@@ -3763,8 +4157,11 @@
       <c r="E118" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119">
         <v>1.38</v>
       </c>
@@ -3780,8 +4177,11 @@
       <c r="E119" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120">
         <v>71.16</v>
       </c>
@@ -3797,8 +4197,11 @@
       <c r="E120" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121">
         <v>8.6199999999999992</v>
       </c>
@@ -3814,8 +4217,11 @@
       <c r="E121" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122">
         <v>12.06</v>
       </c>
@@ -3831,8 +4237,11 @@
       <c r="E122" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123">
         <v>22.08</v>
       </c>
@@ -3848,8 +4257,11 @@
       <c r="E123" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124">
         <v>8.61</v>
       </c>
@@ -3865,8 +4277,11 @@
       <c r="E124" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125">
         <v>12.97</v>
       </c>
@@ -3882,8 +4297,11 @@
       <c r="E125" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126">
         <v>2.08</v>
       </c>
@@ -3899,8 +4317,11 @@
       <c r="E126" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127">
         <v>-100</v>
       </c>
@@ -3916,8 +4337,11 @@
       <c r="E127" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F127" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128">
         <v>3.03</v>
       </c>
@@ -3933,8 +4357,11 @@
       <c r="E128" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129">
         <v>39.64</v>
       </c>
@@ -3950,8 +4377,11 @@
       <c r="E129" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130">
         <v>10.9</v>
       </c>
@@ -3967,8 +4397,11 @@
       <c r="E130" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131">
         <v>76.86</v>
       </c>
@@ -3984,8 +4417,11 @@
       <c r="E131" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132">
         <v>62.86</v>
       </c>
@@ -4001,8 +4437,11 @@
       <c r="E132" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133">
         <v>29.99</v>
       </c>
@@ -4018,8 +4457,11 @@
       <c r="E133" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134">
         <v>1.65</v>
       </c>
@@ -4035,8 +4477,11 @@
       <c r="E134" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135">
         <v>73.72</v>
       </c>
@@ -4052,8 +4497,11 @@
       <c r="E135" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136">
         <v>12.22</v>
       </c>
@@ -4069,8 +4517,11 @@
       <c r="E136" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137">
         <v>8.33</v>
       </c>
@@ -4086,8 +4537,11 @@
       <c r="E137" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138">
         <v>28.85</v>
       </c>
@@ -4103,8 +4557,11 @@
       <c r="E138" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139">
         <v>50.36</v>
       </c>
@@ -4120,8 +4577,11 @@
       <c r="E139" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F139" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140">
         <v>79.58</v>
       </c>
@@ -4137,8 +4597,11 @@
       <c r="E140" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141">
         <v>80.31</v>
       </c>
@@ -4154,8 +4617,11 @@
       <c r="E141" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142">
         <v>3.01</v>
       </c>
@@ -4171,8 +4637,11 @@
       <c r="E142" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143">
         <v>0.48</v>
       </c>
@@ -4188,8 +4657,11 @@
       <c r="E143" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144">
         <v>61.36</v>
       </c>
@@ -4205,8 +4677,11 @@
       <c r="E144" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145">
         <v>0.1</v>
       </c>
@@ -4222,8 +4697,11 @@
       <c r="E145" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F145" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146">
         <v>41.56</v>
       </c>
@@ -4239,8 +4717,11 @@
       <c r="E146" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F146" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147">
         <v>0.87</v>
       </c>
@@ -4256,8 +4737,11 @@
       <c r="E147" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F147" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148">
         <v>27.96</v>
       </c>
@@ -4273,8 +4757,11 @@
       <c r="E148" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F148" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149">
         <v>54.5</v>
       </c>
@@ -4290,8 +4777,11 @@
       <c r="E149" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F149" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150">
         <v>58.82</v>
       </c>
@@ -4307,8 +4797,11 @@
       <c r="E150" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F150" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151">
         <v>30.56</v>
       </c>
@@ -4324,8 +4817,11 @@
       <c r="E151" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F151" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152">
         <v>28.03</v>
       </c>
@@ -4341,8 +4837,11 @@
       <c r="E152" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F152" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
       <c r="A153">
         <v>15.2</v>
       </c>
@@ -4358,8 +4857,11 @@
       <c r="E153" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F153" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154">
         <v>32.33</v>
       </c>
@@ -4375,8 +4877,11 @@
       <c r="E154" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F154" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155">
         <v>2.57</v>
       </c>
@@ -4392,8 +4897,11 @@
       <c r="E155" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F155" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156">
         <v>0.03</v>
       </c>
@@ -4409,8 +4917,11 @@
       <c r="E156" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F156" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157">
         <v>3.65</v>
       </c>
@@ -4426,8 +4937,11 @@
       <c r="E157" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F157" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158">
         <v>21.43</v>
       </c>
@@ -4443,8 +4957,11 @@
       <c r="E158" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F158" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
       <c r="A159">
         <v>23.58</v>
       </c>
@@ -4460,8 +4977,11 @@
       <c r="E159" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F159" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
       <c r="A160">
         <v>3.54</v>
       </c>
@@ -4477,8 +4997,11 @@
       <c r="E160" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F160" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
       <c r="A161">
         <v>79.37</v>
       </c>
@@ -4494,8 +5017,11 @@
       <c r="E161" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F161" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
       <c r="A162">
         <v>1.64</v>
       </c>
@@ -4511,8 +5037,11 @@
       <c r="E162" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F162" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
       <c r="A163">
         <v>9.67</v>
       </c>
@@ -4528,8 +5057,11 @@
       <c r="E163" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F163" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164">
         <v>-100</v>
       </c>
@@ -4545,8 +5077,11 @@
       <c r="E164" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F164" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
       <c r="A165">
         <v>4.9800000000000004</v>
       </c>
@@ -4562,8 +5097,11 @@
       <c r="E165" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F165" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
       <c r="A166">
         <v>35.950000000000003</v>
       </c>
@@ -4579,8 +5117,11 @@
       <c r="E166" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F166" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
       <c r="A167">
         <v>-100</v>
       </c>
@@ -4596,8 +5137,11 @@
       <c r="E167" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F167" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168">
         <v>40.75</v>
       </c>
@@ -4613,8 +5157,11 @@
       <c r="E168" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F168" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
       <c r="A169">
         <v>0.08</v>
       </c>
@@ -4630,8 +5177,11 @@
       <c r="E169" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F169" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
       <c r="A170">
         <v>35.42</v>
       </c>
@@ -4647,8 +5197,11 @@
       <c r="E170" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F170" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
       <c r="A171">
         <v>27.2</v>
       </c>
@@ -4664,8 +5217,11 @@
       <c r="E171" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F171" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
       <c r="A172">
         <v>1.72</v>
       </c>
@@ -4681,8 +5237,11 @@
       <c r="E172" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F172" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173">
         <v>71.14</v>
       </c>
@@ -4698,8 +5257,11 @@
       <c r="E173" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F173" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
       <c r="A174">
         <v>1.1000000000000001</v>
       </c>
@@ -4715,8 +5277,11 @@
       <c r="E174" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175">
         <v>0.05</v>
       </c>
@@ -4732,8 +5297,11 @@
       <c r="E175" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176">
         <v>17.899999999999999</v>
       </c>
@@ -4749,8 +5317,11 @@
       <c r="E176" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F176" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
       <c r="A177">
         <v>23.39</v>
       </c>
@@ -4766,8 +5337,11 @@
       <c r="E177" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F177" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
       <c r="A178">
         <v>49.13</v>
       </c>
@@ -4783,8 +5357,11 @@
       <c r="E178" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F178" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179">
         <v>95.37</v>
       </c>
@@ -4800,8 +5377,11 @@
       <c r="E179" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F179" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
       <c r="A180">
         <v>9.6999999999999993</v>
       </c>
@@ -4817,8 +5397,11 @@
       <c r="E180" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F180" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181">
         <v>32.39</v>
       </c>
@@ -4834,8 +5417,11 @@
       <c r="E181" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F181" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
       <c r="A182">
         <v>18.96</v>
       </c>
@@ -4851,8 +5437,11 @@
       <c r="E182" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F182" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
       <c r="A183">
         <v>48.8</v>
       </c>
@@ -4868,8 +5457,11 @@
       <c r="E183" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F183" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
       <c r="A184">
         <v>15.4</v>
       </c>
@@ -4885,8 +5477,11 @@
       <c r="E184" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F184" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
       <c r="A185">
         <v>60.98</v>
       </c>
@@ -4902,8 +5497,11 @@
       <c r="E185" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F185" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
       <c r="A186">
         <v>14.49</v>
       </c>
@@ -4919,8 +5517,11 @@
       <c r="E186" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F186" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
       <c r="A187">
         <v>57.9</v>
       </c>
@@ -4936,8 +5537,11 @@
       <c r="E187" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F187" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
       <c r="A188">
         <v>27.69</v>
       </c>
@@ -4953,8 +5557,11 @@
       <c r="E188" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F188" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
       <c r="A189">
         <v>1.1399999999999999</v>
       </c>
@@ -4970,8 +5577,11 @@
       <c r="E189" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F189" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
       <c r="A190">
         <v>34.89</v>
       </c>
@@ -4987,8 +5597,11 @@
       <c r="E190" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F190" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
       <c r="A191">
         <v>18.97</v>
       </c>
@@ -5004,8 +5617,11 @@
       <c r="E191" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F191" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
       <c r="A192">
         <v>12.14</v>
       </c>
@@ -5021,8 +5637,11 @@
       <c r="E192" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F192" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193">
         <v>75.13</v>
       </c>
@@ -5038,8 +5657,11 @@
       <c r="E193" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F193" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
       <c r="A194">
         <v>1.77</v>
       </c>
@@ -5055,8 +5677,11 @@
       <c r="E194" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F194" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
       <c r="A195">
         <v>0.46</v>
       </c>
@@ -5072,8 +5697,11 @@
       <c r="E195" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F195" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196">
         <v>11.58</v>
       </c>
@@ -5089,8 +5717,11 @@
       <c r="E196" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F196" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
       <c r="A197">
         <v>12.02</v>
       </c>
@@ -5106,8 +5737,11 @@
       <c r="E197" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F197" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
       <c r="A198">
         <v>0.06</v>
       </c>
@@ -5123,8 +5757,11 @@
       <c r="E198" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F198" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
       <c r="A199">
         <v>0.76</v>
       </c>
@@ -5140,8 +5777,11 @@
       <c r="E199" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F199" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
       <c r="A200">
         <v>5.04</v>
       </c>
@@ -5157,8 +5797,11 @@
       <c r="E200" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F200" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
       <c r="A201">
         <v>90.95</v>
       </c>
@@ -5174,8 +5817,11 @@
       <c r="E201" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F201" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
       <c r="A202">
         <v>8.8699999999999992</v>
       </c>
@@ -5191,8 +5837,11 @@
       <c r="E202" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F202" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6">
       <c r="A203">
         <v>1.01</v>
       </c>
@@ -5208,8 +5857,11 @@
       <c r="E203" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F203" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
       <c r="A204">
         <v>12.15</v>
       </c>
@@ -5225,8 +5877,11 @@
       <c r="E204" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F204" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
       <c r="A205">
         <v>78.31</v>
       </c>
@@ -5242,8 +5897,11 @@
       <c r="E205" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F205" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
       <c r="A206">
         <v>10.9</v>
       </c>
@@ -5259,8 +5917,11 @@
       <c r="E206" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F206" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
       <c r="A207">
         <v>5.9</v>
       </c>
@@ -5276,8 +5937,11 @@
       <c r="E207" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F207" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
       <c r="A208">
         <v>57.8</v>
       </c>
@@ -5293,8 +5957,11 @@
       <c r="E208" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F208" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
       <c r="A209">
         <v>1</v>
       </c>
@@ -5310,8 +5977,11 @@
       <c r="E209" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F209" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6">
       <c r="A210">
         <v>24.64</v>
       </c>
@@ -5327,8 +5997,11 @@
       <c r="E210" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F210" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6">
       <c r="A211">
         <v>33.69</v>
       </c>
@@ -5344,8 +6017,11 @@
       <c r="E211" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F211" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6">
       <c r="A212">
         <v>24.23</v>
       </c>
@@ -5361,8 +6037,11 @@
       <c r="E212" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F212" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6">
       <c r="A213">
         <v>3.67</v>
       </c>
@@ -5378,8 +6057,11 @@
       <c r="E213" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F213" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6">
       <c r="A214">
         <v>83.04</v>
       </c>
@@ -5395,8 +6077,11 @@
       <c r="E214" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F214" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6">
       <c r="A215">
         <v>82.38</v>
       </c>
@@ -5412,8 +6097,11 @@
       <c r="E215" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F215" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6">
       <c r="A216">
         <v>23.99</v>
       </c>
@@ -5429,8 +6117,11 @@
       <c r="E216" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F216" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6">
       <c r="A217">
         <v>19.48</v>
       </c>
@@ -5446,8 +6137,11 @@
       <c r="E217" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F217" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
       <c r="A218">
         <v>4.41</v>
       </c>
@@ -5463,8 +6157,11 @@
       <c r="E218" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F218" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
       <c r="A219">
         <v>58.17</v>
       </c>
@@ -5475,10 +6172,13 @@
         <v>384</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="E219" t="s">
         <v>438</v>
+      </c>
+      <c r="F219" s="5" t="s">
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -5486,5 +6186,6 @@
     <sortCondition ref="D2:D249"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added GDP to simplified data
</commit_message>
<xml_diff>
--- a/data/simplifiedData2021.xlsx
+++ b/data/simplifiedData2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinegorey/Documents/COSI116A/cosi-116a-f24-final-project-repository/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanscassellati/Data_Visualization/Project/cosi-116a-f24-final-project-repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF36A765-B57A-6A45-AA2F-27D1D02261DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121D0C2E-474E-7341-956B-BEB85D11B4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7980" yWindow="2040" windowWidth="13820" windowHeight="14340" xr2:uid="{28DD3533-A644-B740-9E1F-02EA1467CA1F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="449">
   <si>
     <t>Renewable2021</t>
   </si>
@@ -1380,13 +1380,16 @@
   </si>
   <si>
     <t>Continent</t>
+  </si>
+  <si>
+    <t>GDP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1409,12 +1412,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -1445,13 +1442,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1786,22 +1782,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541C9CC-3DC3-A74E-9432-2834F1B0C62F}">
-  <dimension ref="A1:F219"/>
+  <dimension ref="A1:G219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1817,11 +1813,14 @@
       <c r="E1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>19.98</v>
       </c>
@@ -1837,11 +1836,14 @@
       <c r="E2" t="s">
         <v>218</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>378.08289188730799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>41.91</v>
       </c>
@@ -1857,11 +1859,14 @@
       <c r="E3" t="s">
         <v>219</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>6281.0467753941602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.12</v>
       </c>
@@ -1877,11 +1882,14 @@
       <c r="E4" t="s">
         <v>220</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>3700.32056196134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.39</v>
       </c>
@@ -1897,11 +1905,14 @@
       <c r="E5" t="s">
         <v>221</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>18.39</v>
       </c>
@@ -1917,11 +1928,14 @@
       <c r="E6" t="s">
         <v>222</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>42065.970755515402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>52.88</v>
       </c>
@@ -1937,11 +1951,14 @@
       <c r="E7" t="s">
         <v>223</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>2026.03095186582</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.77</v>
       </c>
@@ -1957,11 +1974,14 @@
       <c r="E8" t="s">
         <v>224</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>19106.060926666501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.9</v>
       </c>
@@ -1977,11 +1997,14 @@
       <c r="E9" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>16740.348196381801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9.24</v>
       </c>
@@ -1997,11 +2020,14 @@
       <c r="E10" t="s">
         <v>226</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>10775.9998364776</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9.1300000000000008</v>
       </c>
@@ -2017,11 +2043,14 @@
       <c r="E11" t="s">
         <v>227</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>4972.7864121196399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8.76</v>
       </c>
@@ -2037,11 +2066,14 @@
       <c r="E12" t="s">
         <v>228</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>29127.759385715599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12.32</v>
       </c>
@@ -2057,11 +2089,14 @@
       <c r="E13" t="s">
         <v>229</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>67616.301207924495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>36</v>
       </c>
@@ -2077,11 +2112,14 @@
       <c r="E14" t="s">
         <v>230</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>53720.125274240498</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1.32</v>
       </c>
@@ -2097,11 +2135,14 @@
       <c r="E15" t="s">
         <v>231</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>5316.1499363817902</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1.1100000000000001</v>
       </c>
@@ -2117,11 +2158,14 @@
       <c r="E16" t="s">
         <v>232</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>28260.367047800199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.02</v>
       </c>
@@ -2137,11 +2181,14 @@
       <c r="E17" t="s">
         <v>233</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>26860.074553837701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>25.04</v>
       </c>
@@ -2157,11 +2204,14 @@
       <c r="E18" t="s">
         <v>234</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>2449.0249775325801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5.46</v>
       </c>
@@ -2177,11 +2227,14 @@
       <c r="E19" t="s">
         <v>235</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>17507.4679943101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8.2200000000000006</v>
       </c>
@@ -2197,11 +2250,14 @@
       <c r="E20" t="s">
         <v>236</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>7274.2274848062998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>11.68</v>
       </c>
@@ -2217,11 +2273,14 @@
       <c r="E21" t="s">
         <v>237</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>51737.760268709702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>26.56</v>
       </c>
@@ -2237,11 +2296,14 @@
       <c r="E22" t="s">
         <v>238</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>6060.9682237126599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>54.52</v>
       </c>
@@ -2257,11 +2319,14 @@
       <c r="E23" t="s">
         <v>239</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>1360.9114742179199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.9</v>
       </c>
@@ -2277,11 +2342,14 @@
       <c r="E24" t="s">
         <v>240</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>113524.811092934</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>81.81</v>
       </c>
@@ -2297,11 +2365,14 @@
       <c r="E25" t="s">
         <v>241</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>3560.19789375963</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>12.76</v>
       </c>
@@ -2317,11 +2388,14 @@
       <c r="E26" t="s">
         <v>242</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>3345.0230022656901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>36.61</v>
       </c>
@@ -2337,11 +2411,14 @@
       <c r="E27" t="s">
         <v>243</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>7237.2737869309503</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27.36</v>
       </c>
@@ -2357,11 +2434,14 @@
       <c r="E28" t="s">
         <v>244</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>7238.7960959064703</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>46.48</v>
       </c>
@@ -2377,11 +2457,14 @@
       <c r="E29" t="s">
         <v>245</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>7696.7851302935997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.03</v>
       </c>
@@ -2397,11 +2480,14 @@
       <c r="E30" t="s">
         <v>246</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>31448.9136081385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20.38</v>
       </c>
@@ -2417,11 +2503,14 @@
       <c r="E31" t="s">
         <v>247</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>12204.3686269019</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>71.16</v>
       </c>
@@ -2437,11 +2526,14 @@
       <c r="E32" t="s">
         <v>248</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>904.474929980056</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>83.14</v>
       </c>
@@ -2457,11 +2549,14 @@
       <c r="E33" t="s">
         <v>249</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>298.17034937456702</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>22.64</v>
       </c>
@@ -2477,11 +2572,14 @@
       <c r="E34" t="s">
         <v>250</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>3557.8377753914001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>52.38</v>
       </c>
@@ -2497,11 +2595,14 @@
       <c r="E35" t="s">
         <v>251</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>1625.23502116229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>79.239999999999995</v>
       </c>
@@ -2517,11 +2618,14 @@
       <c r="E36" t="s">
         <v>252</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>1666.93280948232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>23.84</v>
       </c>
@@ -2537,11 +2641,14 @@
       <c r="E37" t="s">
         <v>253</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>52456.719065477497</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.01</v>
       </c>
@@ -2557,11 +2664,14 @@
       <c r="E38" t="s">
         <v>254</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>88475.602352567905</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>90.92</v>
       </c>
@@ -2577,11 +2687,14 @@
       <c r="E39" t="s">
         <v>255</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>461.26499740753502</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>69.900000000000006</v>
       </c>
@@ -2597,11 +2710,14 @@
       <c r="E40" t="s">
         <v>256</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>954.71159725193195</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>24.17</v>
       </c>
@@ -2617,11 +2733,14 @@
       <c r="E41" t="s">
         <v>257</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>16247.401015076701</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>15.21</v>
       </c>
@@ -2637,11 +2756,14 @@
       <c r="E42" t="s">
         <v>258</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>12497.7495022401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>29.7</v>
       </c>
@@ -2657,11 +2779,14 @@
       <c r="E43" t="s">
         <v>259</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>6183.7877829805702</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>41.19</v>
       </c>
@@ -2677,11 +2802,14 @@
       <c r="E44" t="s">
         <v>260</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>1577.4708406611801</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>71.38</v>
       </c>
@@ -2697,11 +2825,14 @@
       <c r="E45" t="s">
         <v>262</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>2525.39450894634</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>8.76</v>
       </c>
@@ -2717,11 +2848,14 @@
       <c r="E46" t="s">
         <v>263</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>14526.1503742855</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>34.159999999999997</v>
       </c>
@@ -2737,11 +2871,14 @@
       <c r="E47" t="s">
         <v>264</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>12537.256746188101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>34.07</v>
       </c>
@@ -2757,11 +2894,14 @@
       <c r="E48" t="s">
         <v>265</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <v>17042.057124043899</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>20.91</v>
       </c>
@@ -2777,11 +2917,14 @@
       <c r="E49" t="s">
         <v>266</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>11255.2293626223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2.75</v>
       </c>
@@ -2797,11 +2940,14 @@
       <c r="E50" t="s">
         <v>267</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>14393.3127372177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>15.63</v>
       </c>
@@ -2817,11 +2963,14 @@
       <c r="E51" t="s">
         <v>268</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <v>33502.203740662699</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>17.16</v>
       </c>
@@ -2837,11 +2986,14 @@
       <c r="E52" t="s">
         <v>269</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <v>26809.808215140802</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>14.72</v>
       </c>
@@ -2857,11 +3009,14 @@
       <c r="E53" t="s">
         <v>320</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <v>654.14800758035506</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>96.33</v>
       </c>
@@ -2877,11 +3032,14 @@
       <c r="E54" t="s">
         <v>261</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <v>551.126915503276</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>39.520000000000003</v>
       </c>
@@ -2897,11 +3055,14 @@
       <c r="E55" t="s">
         <v>270</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <v>69298.149521148996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>26.56</v>
       </c>
@@ -2917,11 +3078,14 @@
       <c r="E56" t="s">
         <v>271</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <v>3348.0133913473601</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>8.83</v>
       </c>
@@ -2937,11 +3101,14 @@
       <c r="E57" t="s">
         <v>272</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <v>7668.1581321696203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>14.82</v>
       </c>
@@ -2957,11 +3124,14 @@
       <c r="E58" t="s">
         <v>273</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <v>8476.7496882799805</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>18.899999999999999</v>
       </c>
@@ -2977,11 +3147,14 @@
       <c r="E59" t="s">
         <v>274</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <v>5965.1328705441601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>6.11</v>
       </c>
@@ -2997,11 +3170,14 @@
       <c r="E60" t="s">
         <v>275</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <v>3898.0197303003501</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>21.91</v>
       </c>
@@ -3017,11 +3193,14 @@
       <c r="E61" t="s">
         <v>276</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <v>4664.31250250429</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>5.25</v>
       </c>
@@ -3037,11 +3216,14 @@
       <c r="E62" t="s">
         <v>277</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <v>7506.66786103709</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>80.66</v>
       </c>
@@ -3057,11 +3239,14 @@
       <c r="E63" t="s">
         <v>278</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <v>610.98435639808497</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>37.979999999999997</v>
       </c>
@@ -3077,11 +3262,14 @@
       <c r="E64" t="s">
         <v>279</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <v>27990.6210290954</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>65.400000000000006</v>
       </c>
@@ -3097,11 +3285,14 @@
       <c r="E65" t="s">
         <v>280</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <v>3978.3940740109401</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>90.63</v>
       </c>
@@ -3117,11 +3308,14 @@
       <c r="E66" t="s">
         <v>281</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <v>825.22212764963103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>5.08</v>
       </c>
@@ -3137,11 +3331,14 @@
       <c r="E67" t="s">
         <v>282</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>29.7</v>
       </c>
@@ -3157,11 +3354,14 @@
       <c r="E68" t="s">
         <v>283</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <v>4656.0505920088499</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>50.22</v>
       </c>
@@ -3177,11 +3377,14 @@
       <c r="E69" t="s">
         <v>284</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <v>53608.593875420403</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>16.25</v>
       </c>
@@ -3197,11 +3400,14 @@
       <c r="E70" t="s">
         <v>285</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <v>44251.465347687401</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>7.44</v>
       </c>
@@ -3217,11 +3423,14 @@
       <c r="E71" t="s">
         <v>286</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <v>20230.241135251301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>91.27</v>
       </c>
@@ -3237,11 +3446,14 @@
       <c r="E72" t="s">
         <v>287</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <v>8635.3567420191594</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>48.58</v>
       </c>
@@ -3257,11 +3469,14 @@
       <c r="E73" t="s">
         <v>288</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <v>776.12730332921501</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>25.18</v>
       </c>
@@ -3277,11 +3492,14 @@
       <c r="E74" t="s">
         <v>289</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <v>4956.2686976539399</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>17.61</v>
       </c>
@@ -3297,11 +3515,14 @@
       <c r="E75" t="s">
         <v>290</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F75" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <v>51295.745214451897</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>39.049999999999997</v>
       </c>
@@ -3317,11 +3538,14 @@
       <c r="E76" t="s">
         <v>291</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <v>2422.0859129289001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>0</v>
       </c>
@@ -3337,11 +3561,14 @@
       <c r="E77" t="s">
         <v>292</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>21.47</v>
       </c>
@@ -3357,11 +3584,14 @@
       <c r="E78" t="s">
         <v>293</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <v>20551.489339166401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>11.64</v>
       </c>
@@ -3377,11 +3607,14 @@
       <c r="E79" t="s">
         <v>294</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F79" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <v>57532.6611638455</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>10.220000000000001</v>
       </c>
@@ -3397,11 +3630,14 @@
       <c r="E80" t="s">
         <v>295</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <v>9010.6707534916295</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>4.5</v>
       </c>
@@ -3417,11 +3653,14 @@
       <c r="E81" t="s">
         <v>296</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F81" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>62.13</v>
       </c>
@@ -3437,11 +3676,14 @@
       <c r="E82" t="s">
         <v>297</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="F82" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82">
+        <v>4887.0240420423597</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>66.849999999999994</v>
       </c>
@@ -3457,11 +3699,14 @@
       <c r="E83" t="s">
         <v>298</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F83" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83">
+        <v>1166.74024776689</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>87.37</v>
       </c>
@@ -3477,11 +3722,14 @@
       <c r="E84" t="s">
         <v>299</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F84" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84">
+        <v>768.66614793675899</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>13.2</v>
       </c>
@@ -3497,11 +3745,14 @@
       <c r="E85" t="s">
         <v>300</v>
       </c>
-      <c r="F85" s="5" t="s">
+      <c r="F85" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85">
+        <v>9994.6457042256898</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>76.72</v>
       </c>
@@ -3517,11 +3768,14 @@
       <c r="E86" t="s">
         <v>301</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F86" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86">
+        <v>1663.5616943561699</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>45.91</v>
       </c>
@@ -3537,11 +3791,14 @@
       <c r="E87" t="s">
         <v>302</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F87" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87">
+        <v>2771.72261645247</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>0.42</v>
       </c>
@@ -3557,11 +3814,14 @@
       <c r="E88" t="s">
         <v>303</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F88" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88">
+        <v>49223.453927734401</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>15.3</v>
       </c>
@@ -3577,11 +3837,14 @@
       <c r="E89" t="s">
         <v>304</v>
       </c>
-      <c r="F89" s="5" t="s">
+      <c r="F89" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89">
+        <v>18753.249737663598</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>82.43</v>
       </c>
@@ -3597,11 +3860,14 @@
       <c r="E90" t="s">
         <v>305</v>
       </c>
-      <c r="F90" s="5" t="s">
+      <c r="F90" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90">
+        <v>69115.639001411895</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>34.92</v>
       </c>
@@ -3617,11 +3883,14 @@
       <c r="E91" t="s">
         <v>306</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F91" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91">
+        <v>2255.8666848583298</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>20.190000000000001</v>
       </c>
@@ -3637,11 +3906,14 @@
       <c r="E92" t="s">
         <v>307</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F92" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92">
+        <v>4334.2159826031402</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>0.91</v>
       </c>
@@ -3657,11 +3929,14 @@
       <c r="E93" t="s">
         <v>308</v>
       </c>
-      <c r="F93" s="5" t="s">
+      <c r="F93" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93">
+        <v>4075.4863437444301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1.1000000000000001</v>
       </c>
@@ -3677,11 +3952,14 @@
       <c r="E94" t="s">
         <v>309</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F94" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94">
+        <v>4770.835339579</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>12.69</v>
       </c>
@@ -3697,11 +3975,14 @@
       <c r="E95" t="s">
         <v>310</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F95" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95">
+        <v>102955.801069294</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>3.16</v>
       </c>
@@ -3717,11 +3998,14 @@
       <c r="E96" t="s">
         <v>311</v>
       </c>
-      <c r="F96" s="5" t="s">
+      <c r="F96" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>6.2</v>
       </c>
@@ -3737,11 +4021,14 @@
       <c r="E97" t="s">
         <v>312</v>
       </c>
-      <c r="F97" s="5" t="s">
+      <c r="F97" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97">
+        <v>55023.230066005897</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>17.54</v>
       </c>
@@ -3757,11 +4044,14 @@
       <c r="E98" t="s">
         <v>313</v>
       </c>
-      <c r="F98" s="5" t="s">
+      <c r="F98" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98">
+        <v>36383.327631384796</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>10.49</v>
       </c>
@@ -3777,11 +4067,14 @@
       <c r="E99" t="s">
         <v>314</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="F99" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99">
+        <v>5183.5801415757896</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>8.84</v>
       </c>
@@ -3797,11 +4090,14 @@
       <c r="E100" t="s">
         <v>315</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="F100" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100">
+        <v>40168.807557252003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>11.5</v>
       </c>
@@ -3817,11 +4113,14 @@
       <c r="E101" t="s">
         <v>316</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="F101" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101">
+        <v>4046.98388472648</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1.99</v>
       </c>
@@ -3837,11 +4136,14 @@
       <c r="E102" t="s">
         <v>317</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="F102" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102">
+        <v>10268.1538168935</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>67.67</v>
       </c>
@@ -3857,11 +4159,14 @@
       <c r="E103" t="s">
         <v>318</v>
       </c>
-      <c r="F103" s="5" t="s">
+      <c r="F103" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103">
+        <v>2069.6611365141798</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>42.23</v>
       </c>
@@ -3877,11 +4182,14 @@
       <c r="E104" t="s">
         <v>319</v>
       </c>
-      <c r="F104" s="5" t="s">
+      <c r="F104" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104">
+        <v>1764.93448610105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -3897,11 +4205,14 @@
       <c r="E105" t="s">
         <v>322</v>
       </c>
-      <c r="F105" s="5" t="s">
+      <c r="F105" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105">
+        <v>32324.602843669101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>27.63</v>
       </c>
@@ -3917,11 +4228,14 @@
       <c r="E106" t="s">
         <v>323</v>
       </c>
-      <c r="F106" s="5" t="s">
+      <c r="F106" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106">
+        <v>1339.0052104082999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>51.53</v>
       </c>
@@ -3937,11 +4251,14 @@
       <c r="E107" t="s">
         <v>324</v>
       </c>
-      <c r="F107" s="5" t="s">
+      <c r="F107" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="G107">
+        <v>2568.92408238079</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>43.99</v>
       </c>
@@ -3957,11 +4274,14 @@
       <c r="E108" t="s">
         <v>325</v>
       </c>
-      <c r="F108" s="5" t="s">
+      <c r="F108" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="G108">
+        <v>21048.469103751799</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>6.82</v>
       </c>
@@ -3977,11 +4297,14 @@
       <c r="E109" t="s">
         <v>326</v>
       </c>
-      <c r="F109" s="5" t="s">
+      <c r="F109" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="G109">
+        <v>6565.3620031161199</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>33.630000000000003</v>
       </c>
@@ -3997,11 +4320,14 @@
       <c r="E110" t="s">
         <v>327</v>
       </c>
-      <c r="F110" s="5" t="s">
+      <c r="F110" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="G110">
+        <v>1054.9327497341601</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>93.19</v>
       </c>
@@ -4017,11 +4343,14 @@
       <c r="E111" t="s">
         <v>328</v>
       </c>
-      <c r="F111" s="5" t="s">
+      <c r="F111" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="G111">
+        <v>551.39973227640496</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>3.12</v>
       </c>
@@ -4037,11 +4366,14 @@
       <c r="E112" t="s">
         <v>329</v>
       </c>
-      <c r="F112" s="5" t="s">
+      <c r="F112" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="G112">
+        <v>5791.2549764979703</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>53.61</v>
       </c>
@@ -4057,11 +4389,14 @@
       <c r="E113" t="s">
         <v>330</v>
       </c>
-      <c r="F113" s="5" t="s">
+      <c r="F113" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113">
+        <v>197504.58495702199</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>33.22</v>
       </c>
@@ -4077,11 +4412,14 @@
       <c r="E114" t="s">
         <v>331</v>
       </c>
-      <c r="F114" s="5" t="s">
+      <c r="F114" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="G114">
+        <v>23971.044018705699</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>20.51</v>
       </c>
@@ -4097,11 +4435,14 @@
       <c r="E115" t="s">
         <v>332</v>
       </c>
-      <c r="F115" s="5" t="s">
+      <c r="F115" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115">
+        <v>133867.19033767801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>83.61</v>
       </c>
@@ -4117,11 +4458,14 @@
       <c r="E116" t="s">
         <v>333</v>
       </c>
-      <c r="F116" s="5" t="s">
+      <c r="F116" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116">
+        <v>503.35208114478303</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>71.08</v>
       </c>
@@ -4137,11 +4481,14 @@
       <c r="E117" t="s">
         <v>334</v>
       </c>
-      <c r="F117" s="5" t="s">
+      <c r="F117" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="G117">
+        <v>628.69450594716398</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>7.48</v>
       </c>
@@ -4157,11 +4504,14 @@
       <c r="E118" t="s">
         <v>335</v>
       </c>
-      <c r="F118" s="5" t="s">
+      <c r="F118" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="G118">
+        <v>11109.268278688</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1.38</v>
       </c>
@@ -4177,11 +4527,14 @@
       <c r="E119" t="s">
         <v>336</v>
       </c>
-      <c r="F119" s="5" t="s">
+      <c r="F119" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="G119">
+        <v>10076.317259899401</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>71.16</v>
       </c>
@@ -4197,11 +4550,14 @@
       <c r="E120" t="s">
         <v>337</v>
       </c>
-      <c r="F120" s="5" t="s">
+      <c r="F120" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120">
+        <v>881.51008863806999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>8.6199999999999992</v>
       </c>
@@ -4217,11 +4573,14 @@
       <c r="E121" t="s">
         <v>338</v>
       </c>
-      <c r="F121" s="5" t="s">
+      <c r="F121" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="G121">
+        <v>34337.433584733502</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>12.06</v>
       </c>
@@ -4237,11 +4596,14 @@
       <c r="E122" t="s">
         <v>339</v>
       </c>
-      <c r="F122" s="5" t="s">
+      <c r="F122" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122">
+        <v>6172.1442568371003</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>22.08</v>
       </c>
@@ -4257,11 +4619,14 @@
       <c r="E123" t="s">
         <v>340</v>
       </c>
-      <c r="F123" s="5" t="s">
+      <c r="F123" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="G123">
+        <v>2166.0447966256002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>8.61</v>
       </c>
@@ -4277,11 +4642,14 @@
       <c r="E124" t="s">
         <v>341</v>
       </c>
-      <c r="F124" s="5" t="s">
+      <c r="F124" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="G124">
+        <v>8835.4000098400393</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>12.97</v>
       </c>
@@ -4297,11 +4665,14 @@
       <c r="E125" t="s">
         <v>342</v>
       </c>
-      <c r="F125" s="5" t="s">
+      <c r="F125" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="G125">
+        <v>10363.1925517983</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2.08</v>
       </c>
@@ -4317,11 +4688,14 @@
       <c r="E126" t="s">
         <v>343</v>
       </c>
-      <c r="F126" s="5" t="s">
+      <c r="F126" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="G126">
+        <v>3571.3367688785602</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>-100</v>
       </c>
@@ -4337,11 +4711,14 @@
       <c r="E127" t="s">
         <v>345</v>
       </c>
-      <c r="F127" s="5" t="s">
+      <c r="F127" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="G127">
+        <v>235132.74555656701</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>3.03</v>
       </c>
@@ -4357,11 +4734,14 @@
       <c r="E128" t="s">
         <v>346</v>
       </c>
-      <c r="F128" s="5" t="s">
+      <c r="F128" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="G128">
+        <v>4566.1401310267502</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>39.64</v>
       </c>
@@ -4377,11 +4757,14 @@
       <c r="E129" t="s">
         <v>347</v>
       </c>
-      <c r="F129" s="5" t="s">
+      <c r="F129" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="G129">
+        <v>9334.2859373043702</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>10.9</v>
       </c>
@@ -4397,11 +4780,14 @@
       <c r="E130" t="s">
         <v>348</v>
       </c>
-      <c r="F130" s="5" t="s">
+      <c r="F130" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="G130">
+        <v>3824.9963023177202</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>76.86</v>
       </c>
@@ -4417,11 +4803,14 @@
       <c r="E131" t="s">
         <v>349</v>
       </c>
-      <c r="F131" s="5" t="s">
+      <c r="F131" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="G131">
+        <v>504.037787154059</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>62.86</v>
       </c>
@@ -4437,11 +4826,14 @@
       <c r="E132" t="s">
         <v>350</v>
       </c>
-      <c r="F132" s="5" t="s">
+      <c r="F132" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="G132">
+        <v>1332.4455771923799</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>29.99</v>
       </c>
@@ -4457,11 +4849,14 @@
       <c r="E133" t="s">
         <v>351</v>
       </c>
-      <c r="F133" s="5" t="s">
+      <c r="F133" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="G133">
+        <v>4919.1889313576403</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>1.65</v>
       </c>
@@ -4477,11 +4872,14 @@
       <c r="E134" t="s">
         <v>352</v>
       </c>
-      <c r="F134" s="5" t="s">
+      <c r="F134" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="G134">
+        <v>12390.370114941899</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>73.72</v>
       </c>
@@ -4497,11 +4895,14 @@
       <c r="E135" t="s">
         <v>353</v>
       </c>
-      <c r="F135" s="5" t="s">
+      <c r="F135" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="G135">
+        <v>1226.70774210372</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>12.22</v>
       </c>
@@ -4517,11 +4918,14 @@
       <c r="E136" t="s">
         <v>354</v>
       </c>
-      <c r="F136" s="5" t="s">
+      <c r="F136" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="G136">
+        <v>58833.060426226199</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>8.33</v>
       </c>
@@ -4537,11 +4941,14 @@
       <c r="E137" t="s">
         <v>355</v>
       </c>
-      <c r="F137" s="5" t="s">
+      <c r="F137" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="G137">
+        <v>34994.265834461701</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>28.85</v>
       </c>
@@ -4557,11 +4964,14 @@
       <c r="E138" t="s">
         <v>356</v>
       </c>
-      <c r="F138" s="5" t="s">
+      <c r="F138" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="G138">
+        <v>49364.707334544699</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>50.36</v>
       </c>
@@ -4577,11 +4987,14 @@
       <c r="E139" t="s">
         <v>357</v>
       </c>
-      <c r="F139" s="5" t="s">
+      <c r="F139" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="140" spans="1:6">
+      <c r="G139">
+        <v>2064.9241659200102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>79.58</v>
       </c>
@@ -4597,11 +5010,14 @@
       <c r="E140" t="s">
         <v>358</v>
       </c>
-      <c r="F140" s="5" t="s">
+      <c r="F140" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="141" spans="1:6">
+      <c r="G140">
+        <v>590.629477265162</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>80.31</v>
       </c>
@@ -4617,11 +5033,14 @@
       <c r="E141" t="s">
         <v>359</v>
       </c>
-      <c r="F141" s="5" t="s">
+      <c r="F141" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="142" spans="1:6">
+      <c r="G141">
+        <v>2019.3137756175199</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>3.01</v>
       </c>
@@ -4637,11 +5056,14 @@
       <c r="E142" t="s">
         <v>360</v>
       </c>
-      <c r="F142" s="5" t="s">
+      <c r="F142" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="143" spans="1:6">
+      <c r="G142">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>0.48</v>
       </c>
@@ -4657,11 +5079,14 @@
       <c r="E143" t="s">
         <v>361</v>
       </c>
-      <c r="F143" s="5" t="s">
+      <c r="F143" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="144" spans="1:6">
+      <c r="G143">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>61.36</v>
       </c>
@@ -4677,11 +5102,14 @@
       <c r="E144" t="s">
         <v>362</v>
       </c>
-      <c r="F144" s="5" t="s">
+      <c r="F144" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="G144">
+        <v>90744.301082150705</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>0.1</v>
       </c>
@@ -4697,11 +5125,14 @@
       <c r="E145" t="s">
         <v>363</v>
       </c>
-      <c r="F145" s="5" t="s">
+      <c r="F145" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="146" spans="1:6">
+      <c r="G145">
+        <v>19509.466486400001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>41.56</v>
       </c>
@@ -4717,11 +5148,14 @@
       <c r="E146" t="s">
         <v>364</v>
       </c>
-      <c r="F146" s="5" t="s">
+      <c r="F146" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="147" spans="1:6">
+      <c r="G146">
+        <v>1480.1107162979399</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>0.87</v>
       </c>
@@ -4737,11 +5171,14 @@
       <c r="E147" t="s">
         <v>365</v>
       </c>
-      <c r="F147" s="5" t="s">
+      <c r="F147" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="148" spans="1:6">
+      <c r="G147">
+        <v>12084.1282734132</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>27.96</v>
       </c>
@@ -4757,11 +5194,14 @@
       <c r="E148" t="s">
         <v>367</v>
       </c>
-      <c r="F148" s="5" t="s">
+      <c r="F148" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="149" spans="1:6">
+      <c r="G148">
+        <v>15491.289790307101</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>54.5</v>
       </c>
@@ -4777,11 +5217,14 @@
       <c r="E149" t="s">
         <v>368</v>
       </c>
-      <c r="F149" s="5" t="s">
+      <c r="F149" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="G149">
+        <v>2624.6041627053901</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>58.82</v>
       </c>
@@ -4797,11 +5240,14 @@
       <c r="E150" t="s">
         <v>369</v>
       </c>
-      <c r="F150" s="5" t="s">
+      <c r="F150" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="G150">
+        <v>5959.44176327886</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>30.56</v>
       </c>
@@ -4817,11 +5263,14 @@
       <c r="E151" t="s">
         <v>370</v>
       </c>
-      <c r="F151" s="5" t="s">
+      <c r="F151" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="152" spans="1:6">
+      <c r="G151">
+        <v>6635.4639234485903</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>28.03</v>
       </c>
@@ -4837,11 +5286,14 @@
       <c r="E152" t="s">
         <v>371</v>
       </c>
-      <c r="F152" s="5" t="s">
+      <c r="F152" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="153" spans="1:6">
+      <c r="G152">
+        <v>3460.5394007761702</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>15.2</v>
       </c>
@@ -4857,11 +5309,14 @@
       <c r="E153" t="s">
         <v>372</v>
       </c>
-      <c r="F153" s="5" t="s">
+      <c r="F153" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="154" spans="1:6">
+      <c r="G153">
+        <v>17786.1284801291</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>32.33</v>
       </c>
@@ -4877,11 +5332,14 @@
       <c r="E154" t="s">
         <v>373</v>
       </c>
-      <c r="F154" s="5" t="s">
+      <c r="F154" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="155" spans="1:6">
+      <c r="G154">
+        <v>24833.0691544972</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>2.57</v>
       </c>
@@ -4897,11 +5355,14 @@
       <c r="E155" t="s">
         <v>374</v>
       </c>
-      <c r="F155" s="5" t="s">
+      <c r="F155" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="156" spans="1:6">
+      <c r="G155">
+        <v>32668.300149752999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>0.03</v>
       </c>
@@ -4917,11 +5378,14 @@
       <c r="E156" t="s">
         <v>375</v>
       </c>
-      <c r="F156" s="5" t="s">
+      <c r="F156" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="157" spans="1:6">
+      <c r="G156">
+        <v>66858.741722708393</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>3.65</v>
       </c>
@@ -4937,11 +5401,14 @@
       <c r="E157" t="s">
         <v>321</v>
       </c>
-      <c r="F157" s="5" t="s">
+      <c r="F157" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="158" spans="1:6">
+      <c r="G157">
+        <v>35084.454623339698</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>21.43</v>
       </c>
@@ -4957,11 +5424,14 @@
       <c r="E158" t="s">
         <v>344</v>
       </c>
-      <c r="F158" s="5" t="s">
+      <c r="F158" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="159" spans="1:6">
+      <c r="G158">
+        <v>4472.2659794730298</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>23.58</v>
       </c>
@@ -4977,11 +5447,14 @@
       <c r="E159" t="s">
         <v>376</v>
       </c>
-      <c r="F159" s="5" t="s">
+      <c r="F159" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="160" spans="1:6">
+      <c r="G159">
+        <v>14786.9430248922</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>3.54</v>
       </c>
@@ -4997,11 +5470,14 @@
       <c r="E160" t="s">
         <v>377</v>
       </c>
-      <c r="F160" s="5" t="s">
+      <c r="F160" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="161" spans="1:6">
+      <c r="G160">
+        <v>12659.2415738744</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>79.37</v>
       </c>
@@ -5017,11 +5493,14 @@
       <c r="E161" t="s">
         <v>378</v>
       </c>
-      <c r="F161" s="5" t="s">
+      <c r="F161" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="162" spans="1:6">
+      <c r="G161">
+        <v>822.31574872768795</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>1.64</v>
       </c>
@@ -5037,11 +5516,14 @@
       <c r="E162" t="s">
         <v>379</v>
       </c>
-      <c r="F162" s="5" t="s">
+      <c r="F162" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="163" spans="1:6">
+      <c r="G162">
+        <v>18082.687989842601</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>9.67</v>
       </c>
@@ -5057,11 +5539,14 @@
       <c r="E163" t="s">
         <v>380</v>
       </c>
-      <c r="F163" s="5" t="s">
+      <c r="F163" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="164" spans="1:6">
+      <c r="G163">
+        <v>9870.7844448196593</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>-100</v>
       </c>
@@ -5077,11 +5562,14 @@
       <c r="E164" t="s">
         <v>381</v>
       </c>
-      <c r="F164" s="5" t="s">
+      <c r="F164" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="165" spans="1:6">
+      <c r="G164">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>4.9800000000000004</v>
       </c>
@@ -5097,11 +5585,14 @@
       <c r="E165" t="s">
         <v>382</v>
       </c>
-      <c r="F165" s="5" t="s">
+      <c r="F165" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="166" spans="1:6">
+      <c r="G165">
+        <v>8360.0997385838109</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>35.950000000000003</v>
       </c>
@@ -5117,11 +5608,14 @@
       <c r="E166" t="s">
         <v>383</v>
       </c>
-      <c r="F166" s="5" t="s">
+      <c r="F166" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="167" spans="1:6">
+      <c r="G166">
+        <v>3918.6597153695602</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>-100</v>
       </c>
@@ -5137,11 +5631,14 @@
       <c r="E167" t="s">
         <v>384</v>
       </c>
-      <c r="F167" s="5" t="s">
+      <c r="F167" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="168" spans="1:6">
+      <c r="G167">
+        <v>54982.832848528502</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>40.75</v>
       </c>
@@ -5157,11 +5654,14 @@
       <c r="E168" t="s">
         <v>385</v>
       </c>
-      <c r="F168" s="5" t="s">
+      <c r="F168" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="169" spans="1:6">
+      <c r="G168">
+        <v>2368.08092859101</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>0.08</v>
       </c>
@@ -5177,11 +5677,14 @@
       <c r="E169" t="s">
         <v>386</v>
       </c>
-      <c r="F169" s="5" t="s">
+      <c r="F169" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="170" spans="1:6">
+      <c r="G169">
+        <v>24160.676045530399</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>35.42</v>
       </c>
@@ -5197,11 +5700,14 @@
       <c r="E170" t="s">
         <v>387</v>
       </c>
-      <c r="F170" s="5" t="s">
+      <c r="F170" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="171" spans="1:6">
+      <c r="G170">
+        <v>1633.56011880605</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>27.2</v>
       </c>
@@ -5217,11 +5723,14 @@
       <c r="E171" t="s">
         <v>388</v>
       </c>
-      <c r="F171" s="5" t="s">
+      <c r="F171" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="172" spans="1:6">
+      <c r="G171">
+        <v>8645.1991011622504</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>1.72</v>
       </c>
@@ -5237,11 +5746,14 @@
       <c r="E172" t="s">
         <v>389</v>
       </c>
-      <c r="F172" s="5" t="s">
+      <c r="F172" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="173" spans="1:6">
+      <c r="G172">
+        <v>14069.590591263501</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>71.14</v>
       </c>
@@ -5257,11 +5769,14 @@
       <c r="E173" t="s">
         <v>390</v>
       </c>
-      <c r="F173" s="5" t="s">
+      <c r="F173" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="174" spans="1:6">
+      <c r="G173">
+        <v>504.621238052416</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1.1000000000000001</v>
       </c>
@@ -5277,11 +5792,14 @@
       <c r="E174" t="s">
         <v>391</v>
       </c>
-      <c r="F174" s="5" t="s">
+      <c r="F174" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="175" spans="1:6">
+      <c r="G174">
+        <v>71333.540901114306</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>0.05</v>
       </c>
@@ -5297,11 +5815,14 @@
       <c r="E175" t="s">
         <v>392</v>
       </c>
-      <c r="F175" s="5" t="s">
+      <c r="F175" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="176" spans="1:6">
+      <c r="G175">
+        <v>31439.009843067499</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>17.899999999999999</v>
       </c>
@@ -5317,11 +5838,14 @@
       <c r="E176" t="s">
         <v>393</v>
       </c>
-      <c r="F176" s="5" t="s">
+      <c r="F176" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="177" spans="1:6">
+      <c r="G176">
+        <v>21766.6502085834</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>23.39</v>
       </c>
@@ -5337,11 +5861,14 @@
       <c r="E177" t="s">
         <v>394</v>
       </c>
-      <c r="F177" s="5" t="s">
+      <c r="F177" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="178" spans="1:6">
+      <c r="G177">
+        <v>29174.252053084801</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>49.13</v>
       </c>
@@ -5357,11 +5884,14 @@
       <c r="E178" t="s">
         <v>395</v>
       </c>
-      <c r="F178" s="5" t="s">
+      <c r="F178" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="179" spans="1:6">
+      <c r="G178">
+        <v>2232.5076572766002</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>95.37</v>
       </c>
@@ -5377,11 +5907,14 @@
       <c r="E179" t="s">
         <v>396</v>
       </c>
-      <c r="F179" s="5" t="s">
+      <c r="F179" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="180" spans="1:6">
+      <c r="G179">
+        <v>576.54058188818794</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>9.6999999999999993</v>
       </c>
@@ -5397,11 +5930,14 @@
       <c r="E180" t="s">
         <v>397</v>
       </c>
-      <c r="F180" s="5" t="s">
+      <c r="F180" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="181" spans="1:6">
+      <c r="G180">
+        <v>7073.6126517293396</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>32.39</v>
       </c>
@@ -5417,11 +5953,14 @@
       <c r="E181" t="s">
         <v>398</v>
       </c>
-      <c r="F181" s="5" t="s">
+      <c r="F181" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="182" spans="1:6">
+      <c r="G181">
+        <v>399.31788910620497</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>18.96</v>
       </c>
@@ -5437,11 +5976,14 @@
       <c r="E182" t="s">
         <v>399</v>
       </c>
-      <c r="F182" s="5" t="s">
+      <c r="F182" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="183" spans="1:6">
+      <c r="G182">
+        <v>30443.1451220136</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>48.8</v>
       </c>
@@ -5457,11 +5999,14 @@
       <c r="E183" t="s">
         <v>400</v>
       </c>
-      <c r="F183" s="5" t="s">
+      <c r="F183" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="184" spans="1:6">
+      <c r="G183">
+        <v>4102.3629044792397</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>15.4</v>
       </c>
@@ -5477,11 +6022,14 @@
       <c r="E184" t="s">
         <v>366</v>
       </c>
-      <c r="F184" s="5" t="s">
+      <c r="F184" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="185" spans="1:6">
+      <c r="G184">
+        <v>3527.6869563049099</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>60.98</v>
       </c>
@@ -5497,11 +6045,14 @@
       <c r="E185" t="s">
         <v>401</v>
       </c>
-      <c r="F185" s="5" t="s">
+      <c r="F185" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="186" spans="1:6">
+      <c r="G185">
+        <v>770.81257426551701</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>14.49</v>
       </c>
@@ -5517,11 +6068,14 @@
       <c r="E186" t="s">
         <v>402</v>
       </c>
-      <c r="F186" s="5" t="s">
+      <c r="F186" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="187" spans="1:6">
+      <c r="G186">
+        <v>5429.6472334222499</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>57.9</v>
       </c>
@@ -5537,11 +6091,14 @@
       <c r="E187" t="s">
         <v>403</v>
       </c>
-      <c r="F187" s="5" t="s">
+      <c r="F187" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="188" spans="1:6">
+      <c r="G187">
+        <v>61116.750524951502</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>27.69</v>
       </c>
@@ -5557,11 +6114,14 @@
       <c r="E188" t="s">
         <v>404</v>
       </c>
-      <c r="F188" s="5" t="s">
+      <c r="F188" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="189" spans="1:6">
+      <c r="G188">
+        <v>93587.710345426094</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>1.1399999999999999</v>
       </c>
@@ -5577,11 +6137,14 @@
       <c r="E189" t="s">
         <v>405</v>
       </c>
-      <c r="F189" s="5" t="s">
+      <c r="F189" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="190" spans="1:6">
+      <c r="G189">
+        <v>556.02237303724598</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>34.89</v>
       </c>
@@ -5597,11 +6160,14 @@
       <c r="E190" t="s">
         <v>406</v>
       </c>
-      <c r="F190" s="5" t="s">
+      <c r="F190" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="191" spans="1:6">
+      <c r="G190">
+        <v>916.69196706192201</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>18.97</v>
       </c>
@@ -5617,11 +6183,14 @@
       <c r="E191" t="s">
         <v>408</v>
       </c>
-      <c r="F191" s="5" t="s">
+      <c r="F191" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="192" spans="1:6">
+      <c r="G191">
+        <v>7060.8980461745105</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>12.14</v>
       </c>
@@ -5637,11 +6206,14 @@
       <c r="E192" t="s">
         <v>409</v>
       </c>
-      <c r="F192" s="5" t="s">
+      <c r="F192" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="193" spans="1:6">
+      <c r="G192">
+        <v>2741.9508290295898</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>75.13</v>
       </c>
@@ -5657,11 +6229,14 @@
       <c r="E193" t="s">
         <v>410</v>
       </c>
-      <c r="F193" s="5" t="s">
+      <c r="F193" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="194" spans="1:6">
+      <c r="G193">
+        <v>959.38148775347997</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>1.77</v>
       </c>
@@ -5677,11 +6252,14 @@
       <c r="E194" t="s">
         <v>411</v>
       </c>
-      <c r="F194" s="5" t="s">
+      <c r="F194" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="195" spans="1:6">
+      <c r="G194">
+        <v>4450.5314926127303</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>0.46</v>
       </c>
@@ -5697,11 +6275,14 @@
       <c r="E195" t="s">
         <v>412</v>
       </c>
-      <c r="F195" s="5" t="s">
+      <c r="F195" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="196" spans="1:6">
+      <c r="G195">
+        <v>16056.230657218501</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>11.58</v>
       </c>
@@ -5717,11 +6298,14 @@
       <c r="E196" t="s">
         <v>413</v>
       </c>
-      <c r="F196" s="5" t="s">
+      <c r="F196" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="197" spans="1:6">
+      <c r="G196">
+        <v>3807.1846538562399</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>12.02</v>
       </c>
@@ -5737,11 +6321,14 @@
       <c r="E197" t="s">
         <v>414</v>
       </c>
-      <c r="F197" s="5" t="s">
+      <c r="F197" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="198" spans="1:6">
+      <c r="G197">
+        <v>9671.0275274001797</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>0.06</v>
       </c>
@@ -5757,11 +6344,14 @@
       <c r="E198" t="s">
         <v>415</v>
       </c>
-      <c r="F198" s="5" t="s">
+      <c r="F198" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="199" spans="1:6">
+      <c r="G198">
+        <v>8803.8092163885794</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>0.76</v>
       </c>
@@ -5777,11 +6367,14 @@
       <c r="E199" t="s">
         <v>416</v>
       </c>
-      <c r="F199" s="5" t="s">
+      <c r="F199" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="200" spans="1:6">
+      <c r="G199">
+        <v>23158.637895110201</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>5.04</v>
       </c>
@@ -5797,11 +6390,14 @@
       <c r="E200" t="s">
         <v>417</v>
       </c>
-      <c r="F200" s="5" t="s">
+      <c r="F200" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="201" spans="1:6">
+      <c r="G200">
+        <v>5370.4192705283604</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>90.95</v>
       </c>
@@ -5817,11 +6413,14 @@
       <c r="E201" t="s">
         <v>418</v>
       </c>
-      <c r="F201" s="5" t="s">
+      <c r="F201" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="202" spans="1:6">
+      <c r="G201">
+        <v>929.68409280180799</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>8.8699999999999992</v>
       </c>
@@ -5837,11 +6436,14 @@
       <c r="E202" t="s">
         <v>419</v>
       </c>
-      <c r="F202" s="5" t="s">
+      <c r="F202" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="203" spans="1:6">
+      <c r="G202">
+        <v>4589.0037032215696</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>1.01</v>
       </c>
@@ -5857,11 +6459,14 @@
       <c r="E203" t="s">
         <v>420</v>
       </c>
-      <c r="F203" s="5" t="s">
+      <c r="F203" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="204" spans="1:6">
+      <c r="G203">
+        <v>44332.3400513046</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>12.15</v>
       </c>
@@ -5877,11 +6482,14 @@
       <c r="E204" t="s">
         <v>421</v>
       </c>
-      <c r="F204" s="5" t="s">
+      <c r="F204" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="205" spans="1:6">
+      <c r="G204">
+        <v>46692.295530969801</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>78.31</v>
       </c>
@@ -5897,11 +6505,14 @@
       <c r="E205" t="s">
         <v>407</v>
       </c>
-      <c r="F205" s="5" t="s">
+      <c r="F205" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="206" spans="1:6">
+      <c r="G205">
+        <v>1151.1832569999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>10.9</v>
       </c>
@@ -5917,11 +6528,14 @@
       <c r="E206" t="s">
         <v>422</v>
       </c>
-      <c r="F206" s="5" t="s">
+      <c r="F206" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="207" spans="1:6">
+      <c r="G206">
+        <v>70012.363054524103</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>5.9</v>
       </c>
@@ -5937,11 +6551,14 @@
       <c r="E207" t="s">
         <v>428</v>
       </c>
-      <c r="F207" s="5" t="s">
+      <c r="F207" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="208" spans="1:6">
+      <c r="G207">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>57.8</v>
       </c>
@@ -5957,11 +6574,14 @@
       <c r="E208" t="s">
         <v>423</v>
       </c>
-      <c r="F208" s="5" t="s">
+      <c r="F208" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="209" spans="1:6">
+      <c r="G208">
+        <v>17923.429479777398</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>1</v>
       </c>
@@ -5977,11 +6597,14 @@
       <c r="E209" t="s">
         <v>424</v>
       </c>
-      <c r="F209" s="5" t="s">
+      <c r="F209" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="210" spans="1:6">
+      <c r="G209">
+        <v>2042.1846097146799</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>24.64</v>
       </c>
@@ -5997,11 +6620,14 @@
       <c r="E210" t="s">
         <v>425</v>
       </c>
-      <c r="F210" s="5" t="s">
+      <c r="F210" s="4" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="211" spans="1:6">
+      <c r="G210">
+        <v>3044.5736403195701</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>33.69</v>
       </c>
@@ -6017,11 +6643,14 @@
       <c r="E211" t="s">
         <v>426</v>
       </c>
-      <c r="F211" s="5" t="s">
+      <c r="F211" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="212" spans="1:6">
+      <c r="G211">
+        <v>3966.6307268595601</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>24.23</v>
       </c>
@@ -6037,11 +6666,14 @@
       <c r="E212" t="s">
         <v>427</v>
       </c>
-      <c r="F212" s="5" t="s">
+      <c r="F212" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="213" spans="1:6">
+      <c r="G212">
+        <v>3756.4889009138601</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>3.67</v>
       </c>
@@ -6057,11 +6689,14 @@
       <c r="E213" t="s">
         <v>429</v>
       </c>
-      <c r="F213" s="5" t="s">
+      <c r="F213" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="214" spans="1:6">
+      <c r="G213">
+        <v>271.99410672045502</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>83.04</v>
       </c>
@@ -6077,11 +6712,14 @@
       <c r="E214" t="s">
         <v>430</v>
       </c>
-      <c r="F214" s="5" t="s">
+      <c r="F214" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="215" spans="1:6">
+      <c r="G214">
+        <v>1135.0782547065501</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>82.38</v>
       </c>
@@ -6097,11 +6735,14 @@
       <c r="E215" t="s">
         <v>431</v>
       </c>
-      <c r="F215" s="5" t="s">
+      <c r="F215" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="216" spans="1:6">
+      <c r="G215">
+        <v>1507.9947898912101</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>23.99</v>
       </c>
@@ -6117,11 +6758,14 @@
       <c r="E216" t="s">
         <v>433</v>
       </c>
-      <c r="F216" s="5" t="s">
+      <c r="F216" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="217" spans="1:6">
+      <c r="G216">
+        <v>5663.0864982068697</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>19.48</v>
       </c>
@@ -6137,11 +6781,14 @@
       <c r="E217" t="s">
         <v>435</v>
       </c>
-      <c r="F217" s="5" t="s">
+      <c r="F217" s="4" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="218" spans="1:6">
+      <c r="G217">
+        <v>6656.2425926810902</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>4.41</v>
       </c>
@@ -6157,11 +6804,14 @@
       <c r="E218" t="s">
         <v>437</v>
       </c>
-      <c r="F218" s="5" t="s">
+      <c r="F218" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="219" spans="1:6">
+      <c r="G218">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>58.17</v>
       </c>
@@ -6177,8 +6827,11 @@
       <c r="E219" t="s">
         <v>438</v>
       </c>
-      <c r="F219" s="5" t="s">
+      <c r="F219" s="4" t="s">
         <v>442</v>
+      </c>
+      <c r="G219">
+        <v>2613.3788930537798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>